<commit_message>
Ajustado o detalhe de numero com virgula nos testes do excel; Alterado pouca coisa nos casos de teste; Alterado boa parte da implementacao na classe alvo
</commit_message>
<xml_diff>
--- a/casos de test.xlsx
+++ b/casos de test.xlsx
@@ -205,6 +205,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">álcool </t>
     </r>
@@ -226,19 +227,19 @@
     <t xml:space="preserve">álcool extra = -1</t>
   </si>
   <si>
-    <t xml:space="preserve">álcool inicial = 600</t>
+    <t xml:space="preserve">álcool inicial = 625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">álcool extra = 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">álcool inicial = 1200</t>
   </si>
   <si>
     <t xml:space="preserve">álcool extra = 300</t>
   </si>
   <si>
-    <t xml:space="preserve">Retorno = 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">álcool inicial = 1200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">álcool extra = 100</t>
+    <t xml:space="preserve">Retorno = 100</t>
   </si>
   <si>
     <t xml:space="preserve">encomendaCombustivel</t>
@@ -256,7 +257,7 @@
     <t xml:space="preserve">Solicitou = 100</t>
   </si>
   <si>
-    <t xml:space="preserve">250; 5030; 625,5; 625,5;</t>
+    <t xml:space="preserve">250; 5030; 625; 625;</t>
   </si>
   <si>
     <t xml:space="preserve">Normal e Posto Emergência pede combustível</t>
@@ -268,7 +269,7 @@
     <t xml:space="preserve">Solicitou = 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">160; 3350; 400,5; 400,5;</t>
+    <t xml:space="preserve">160; 3350; 400; 400;</t>
   </si>
   <si>
     <t xml:space="preserve">Sobreaviso e Posto Comum pede combustível (50%)</t>
@@ -374,6 +375,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -472,20 +474,20 @@
   </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="19.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="99.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="74.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="74.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="50.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="40.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="74.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="50.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="1" width="38.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -888,7 +890,7 @@
         <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>42</v>
@@ -899,13 +901,13 @@
     </row>
     <row r="27" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>46</v>
@@ -1055,7 +1057,7 @@
     </row>
     <row r="40" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1064,7 +1066,7 @@
       </c>
       <c r="B41" s="1" t="n">
         <f aca="false">A41-(A40*0.05)</f>
-        <v>-10</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1073,31 +1075,31 @@
       </c>
       <c r="B42" s="1" t="n">
         <f aca="false">A42-(A40*0.7)</f>
-        <v>860</v>
+        <v>720</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>125</v>
+        <v>638</v>
       </c>
       <c r="B43" s="1" t="n">
-        <f aca="false">A43-(A40*0.25)/2</f>
-        <v>100</v>
+        <f aca="false">A43-(A40*(0.25/2))</f>
+        <v>588</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>125</v>
+        <v>638</v>
       </c>
       <c r="B44" s="1" t="n">
         <f aca="false">A44-(A40*0.25)/2</f>
-        <v>100</v>
+        <v>588</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="19.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(B41,"; ",B42,"; ",B43,"; ",B44,"; ")</f>
-        <v>-10; 860; 100; 100; </v>
+        <v>-20; 720; 588; 588; </v>
       </c>
     </row>
   </sheetData>

</xml_diff>